<commit_message>
updated documents for the week
</commit_message>
<xml_diff>
--- a/bin/Documents/Meeting Log.xlsx
+++ b/bin/Documents/Meeting Log.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -52,13 +52,25 @@
     <t>Revising planning poker, going over deliverables</t>
   </si>
   <si>
-    <t xml:space="preserve">10:50am - </t>
+    <t>10:50am - 11:15</t>
   </si>
   <si>
     <t>Feiyu, Josh</t>
   </si>
   <si>
     <t>Nicole, Jacob</t>
+  </si>
+  <si>
+    <t>CRM, Sprint plan, High Level Design, Project requirements docs</t>
+  </si>
+  <si>
+    <t>11:15-11:30</t>
+  </si>
+  <si>
+    <t>Nicole, Feiyu, Nicole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit testing, System Testing, Bug list, Performance document </t>
   </si>
 </sst>
 </file>
@@ -193,6 +205,26 @@
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>43188.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>